<commit_message>
feature: add sputter equipment
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/zhong_che_zhu_zhou/zhong_che_zhu_zhou_manual.xlsx
+++ b/equipment_cyg/product/zhong_che_zhu_zhou/zhong_che_zhu_zhou_manual.xlsx
@@ -114,7 +114,7 @@
   <si>
     <t>报警/解除报警上报给Host
 alarm_code的数据类型：BINARRY
-alarm_id的数据类型：I4
+alarm_id的数据类型：U4
 alarm_text的数据类型：ASCII</t>
   </si>
   <si>
@@ -3108,7 +3108,7 @@
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>

</xml_diff>